<commit_message>
Reunião do dia 14 de março. Preciso terminar a terceira tabela do BS 1, limpar as tabelas que eu utilizei como exemplo e fazer o BS 2
</commit_message>
<xml_diff>
--- a/Data/out of date/Tabela Resistências.xlsx
+++ b/Data/out of date/Tabela Resistências.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MasterDegreeHCV\Data\out of date\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="204" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="204" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
     <sheet name="Table2" sheetId="3" r:id="rId2"/>
-    <sheet name="Legenda" sheetId="2" r:id="rId3"/>
+    <sheet name="Plan1" sheetId="4" r:id="rId3"/>
+    <sheet name="Plan3" sheetId="6" r:id="rId4"/>
+    <sheet name="Plan2" sheetId="5" r:id="rId5"/>
+    <sheet name="Legenda" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="119">
   <si>
     <t>Variant</t>
   </si>
@@ -296,13 +304,109 @@
   </si>
   <si>
     <t>VEL = velpatasvir</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>OMV</t>
+  </si>
+  <si>
+    <t>PIB</t>
+  </si>
+  <si>
+    <t>EBR</t>
+  </si>
+  <si>
+    <t>VEL</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>DLDV</t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>MXYPST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSIÇÃO28 </t>
+  </si>
+  <si>
+    <t>atg</t>
+  </si>
+  <si>
+    <t>codon resistente 1</t>
+  </si>
+  <si>
+    <t>att</t>
+  </si>
+  <si>
+    <t>posição 30</t>
+  </si>
+  <si>
+    <t>gcg</t>
+  </si>
+  <si>
+    <t>codon resistente 30 -1</t>
+  </si>
+  <si>
+    <t>codon usage 28 - 1</t>
+  </si>
+  <si>
+    <t>freq 28 - 1</t>
+  </si>
+  <si>
+    <t>barreira 28 - 1</t>
+  </si>
+  <si>
+    <t>paciente 1 - input</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>dcv - 0,82</t>
+  </si>
+  <si>
+    <t>ldv - 0,54</t>
+  </si>
+  <si>
+    <t>vel - 0,21</t>
+  </si>
+  <si>
+    <t>Remédio</t>
+  </si>
+  <si>
+    <t>Probabilidade de resistencia</t>
+  </si>
+  <si>
+    <t>ttt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -313,13 +417,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -349,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -369,12 +484,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -699,45 +839,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="18" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
@@ -749,14 +889,14 @@
       <c r="C2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="D2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3"/>
@@ -1234,36 +1374,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A2" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
@@ -1912,16 +2052,1403 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.7265625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>3</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="12">
+        <v>31</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="12">
+        <v>31</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="12">
+        <v>31</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="12">
+        <v>31</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="12">
+        <v>31</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="12">
+        <v>31</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="12">
+        <v>31</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="12">
+        <v>31</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="12">
+        <v>31</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="8" max="8" width="14.90625" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.42</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3">
+        <v>0.4</v>
+      </c>
+      <c r="J3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="E10" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="G11" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="G12" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="G13" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:D43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="12">
+        <v>24</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>28</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>28</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8">
+        <v>30</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8">
+        <v>30</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8">
+        <v>30</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="12">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12">
+        <v>30</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="12">
+        <v>30</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="12">
+        <v>30</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="12">
+        <v>30</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="12">
+        <v>30</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="12">
+        <v>31</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="12">
+        <v>31</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="12">
+        <v>31</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="12">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="12">
+        <v>31</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="12">
+        <v>31</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="12">
+        <v>58</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="12">
+        <v>93</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="12">
+        <v>93</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="12">
+        <v>93</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="12">
+        <v>93</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="12">
+        <v>93</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="12">
+        <v>93</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="12">
+        <v>28</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="12">
+        <v>28</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="12">
+        <v>28</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="12">
+        <v>28</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="12">
+        <v>30</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="12">
+        <v>30</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="12">
+        <v>30</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="12">
+        <v>30</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="12">
+        <v>31</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="12">
+        <v>31</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="12">
+        <v>31</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="12">
+        <v>31</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="12">
+        <v>31</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="12">
+        <v>31</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>

<commit_message>
N sei mais oq fazer...
</commit_message>
<xml_diff>
--- a/Data/out of date/Tabela Resistências.xlsx
+++ b/Data/out of date/Tabela Resistências.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MasterDegreeHCV\Data\out of date\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="204" firstSheet="1" activeTab="2"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
     <sheet name="Table2" sheetId="3" r:id="rId2"/>
     <sheet name="Plan1" sheetId="4" r:id="rId3"/>
-    <sheet name="Plan3" sheetId="6" r:id="rId4"/>
+    <sheet name="Exemplo" sheetId="6" r:id="rId4"/>
     <sheet name="Plan2" sheetId="5" r:id="rId5"/>
     <sheet name="Legenda" sheetId="2" r:id="rId6"/>
   </sheets>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="123">
   <si>
     <t>Variant</t>
   </si>
@@ -400,12 +395,24 @@
   </si>
   <si>
     <t>ttt</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -488,9 +495,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,6 +505,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,45 +846,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1796875" style="2"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
@@ -889,14 +896,14 @@
       <c r="C2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="D2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3"/>
@@ -1374,36 +1381,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:G1048576"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
@@ -2052,25 +2059,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.7265625" style="12"/>
+    <col min="9" max="12" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2092,20 +2099,8 @@
       <c r="G2" s="4">
         <v>3</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="12">
-        <v>31</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -2115,7 +2110,7 @@
       <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
       <c r="E3" s="6">
@@ -2127,20 +2122,8 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="12">
-        <v>31</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -2150,7 +2133,7 @@
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" s="6">
@@ -2162,20 +2145,8 @@
       <c r="G4" s="6">
         <v>0</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="12">
-        <v>31</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -2188,7 +2159,7 @@
       <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>1</v>
       </c>
       <c r="F5" s="6">
@@ -2197,20 +2168,8 @@
       <c r="G5" s="6">
         <v>0</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="12">
-        <v>31</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2232,20 +2191,8 @@
       <c r="G6" s="6">
         <v>0</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="12">
-        <v>31</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -2267,20 +2214,8 @@
       <c r="G7" s="6">
         <v>0</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="12">
-        <v>31</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -2290,7 +2225,7 @@
       <c r="C8" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>1</v>
       </c>
       <c r="E8" s="6">
@@ -2302,20 +2237,8 @@
       <c r="G8" s="6">
         <v>0</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="12">
-        <v>31</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
@@ -2325,7 +2248,7 @@
       <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>1</v>
       </c>
       <c r="E9" s="6">
@@ -2337,20 +2260,8 @@
       <c r="G9" s="6">
         <v>0</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="12">
-        <v>31</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
@@ -2363,7 +2274,7 @@
       <c r="D10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>1</v>
       </c>
       <c r="F10" s="6">
@@ -2372,20 +2283,8 @@
       <c r="G10" s="6">
         <v>0</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="12">
-        <v>31</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
@@ -2404,11 +2303,11 @@
       <c r="F11" s="6">
         <v>0</v>
       </c>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
@@ -2427,11 +2326,11 @@
       <c r="F12" s="6">
         <v>0</v>
       </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
         <v>35</v>
       </c>
@@ -2454,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
@@ -2464,20 +2363,20 @@
       <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10">
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
         <v>1</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
       </c>
-      <c r="G14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
@@ -2490,7 +2389,7 @@
       <c r="D15" s="6">
         <v>0</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>1</v>
       </c>
       <c r="F15" s="6">
@@ -2500,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
@@ -2513,7 +2412,7 @@
       <c r="D16" s="6">
         <v>0</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>1</v>
       </c>
       <c r="F16" s="6">
@@ -2556,7 +2455,7 @@
       <c r="C18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>1</v>
       </c>
       <c r="E18" s="6">
@@ -2582,13 +2481,13 @@
       <c r="D19" s="6">
         <v>0</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="9">
         <v>1</v>
       </c>
       <c r="F19" s="6">
         <v>1</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2605,7 +2504,7 @@
       <c r="D20" s="6">
         <v>0</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="9">
         <v>1</v>
       </c>
       <c r="F20" s="6">
@@ -2628,7 +2527,7 @@
       <c r="D21" s="6">
         <v>0</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="9">
         <v>1</v>
       </c>
       <c r="F21" s="6">
@@ -2648,16 +2547,16 @@
       <c r="C22" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9">
         <v>1</v>
       </c>
       <c r="F22" s="6">
         <v>0</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2690,21 +2589,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" customWidth="1"/>
-    <col min="5" max="5" width="20.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="14.90625" customWidth="1"/>
-    <col min="9" max="9" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2764,7 +2663,7 @@
       <c r="H2" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <v>8.2000000000000007E-3</v>
       </c>
     </row>
@@ -2822,615 +2721,1105 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D43"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12">
+      <c r="B1" s="11">
         <v>24</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8">
         <v>24</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8">
         <v>28</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="8">
         <v>28</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="8">
         <v>28</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="8">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="8">
         <v>30</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="8">
         <v>30</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="8">
         <v>30</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="8">
         <v>30</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="12">
-        <v>30</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="11">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="12">
-        <v>30</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="11">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="12">
-        <v>30</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="B13" s="11">
+        <v>30</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12">
-        <v>30</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="11">
+        <v>30</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="12">
-        <v>30</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="11">
+        <v>30</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="12">
-        <v>30</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="11">
+        <v>30</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>31</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>31</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="11">
         <v>31</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="C19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="11">
         <v>31</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="11">
         <v>31</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="11">
         <v>31</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="11">
         <v>58</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="12">
-        <v>93</v>
-      </c>
-      <c r="C24" s="11" t="s">
+      <c r="B24" s="11">
+        <v>93</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="12">
-        <v>93</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="B25" s="11">
+        <v>93</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="12">
-        <v>93</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="B26" s="11">
+        <v>93</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="12">
-        <v>93</v>
-      </c>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="11">
+        <v>93</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="12">
-        <v>93</v>
-      </c>
-      <c r="C28" s="11" t="s">
+      <c r="B28" s="11">
+        <v>93</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="12">
-        <v>93</v>
-      </c>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="11">
+        <v>93</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="12">
+      <c r="A30" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="11">
         <v>28</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="12">
+      <c r="A31" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="11">
         <v>28</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="12">
+      <c r="A32" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11">
         <v>28</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="11" t="s">
+      <c r="C32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="12">
+      <c r="A33" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="11">
         <v>28</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="12">
-        <v>30</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="A34" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="11">
+        <v>30</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="12">
-        <v>30</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="A35" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="11">
+        <v>30</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="12">
-        <v>30</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="A36" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="11">
+        <v>30</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="12">
-        <v>30</v>
-      </c>
-      <c r="C37" s="11" t="s">
+      <c r="A37" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="11">
+        <v>30</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="12">
+      <c r="A38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="11">
         <v>31</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="12">
+      <c r="A39" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="11">
         <v>31</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="12">
+      <c r="A40" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="11">
         <v>31</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="C40" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="12">
+      <c r="A41" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="11">
         <v>31</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="12">
+      <c r="A42" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="11">
         <v>31</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="12">
+      <c r="A43" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="11">
         <v>31</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="11">
+        <v>31</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="11">
+        <v>31</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="11">
+        <v>31</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="11">
+        <v>31</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="11">
+        <v>31</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="11">
+        <v>31</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="11">
+        <v>31</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="11">
+        <v>31</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="11">
+        <v>31</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="11">
+        <v>58</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="11">
+        <v>58</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="11">
+        <v>92</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="11">
+        <v>93</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="11">
+        <v>93</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="11">
+        <v>93</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="11">
+        <v>93</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="11">
+        <v>93</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="11">
+        <v>93</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="11">
+        <v>3</v>
+      </c>
+      <c r="B62" s="11">
+        <v>30</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="11">
+        <v>3</v>
+      </c>
+      <c r="B63" s="11">
+        <v>30</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="11">
+        <v>3</v>
+      </c>
+      <c r="B64" s="11">
+        <v>30</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="11">
+        <v>3</v>
+      </c>
+      <c r="B65" s="11">
+        <v>30</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="11">
+        <v>3</v>
+      </c>
+      <c r="B66" s="11">
+        <v>31</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="11">
+        <v>3</v>
+      </c>
+      <c r="B67" s="11">
+        <v>31</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="11">
+        <v>3</v>
+      </c>
+      <c r="B68" s="11">
+        <v>31</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="11">
+        <v>3</v>
+      </c>
+      <c r="B69" s="11">
+        <v>31</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="11">
+        <v>3</v>
+      </c>
+      <c r="B70" s="11">
+        <v>31</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="11">
+        <v>3</v>
+      </c>
+      <c r="B71" s="11">
+        <v>31</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="11">
+        <v>3</v>
+      </c>
+      <c r="B72" s="11">
+        <v>58</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="11">
+        <v>3</v>
+      </c>
+      <c r="B73" s="11">
+        <v>93</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="11">
+        <v>3</v>
+      </c>
+      <c r="B74" s="11">
+        <v>93</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="11">
+        <v>3</v>
+      </c>
+      <c r="B75" s="11">
+        <v>93</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="11">
+        <v>3</v>
+      </c>
+      <c r="B76" s="11">
+        <v>93</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="11">
+        <v>3</v>
+      </c>
+      <c r="B77" s="11">
+        <v>93</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="11">
+        <v>3</v>
+      </c>
+      <c r="B78" s="11">
+        <v>93</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3439,16 +3828,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>